<commit_message>
Completed 5th course: AWS QuickSight
</commit_message>
<xml_diff>
--- a/202112_AWS_AssociateDeveloper/AWS_Quicksight.xlsx
+++ b/202112_AWS_AssociateDeveloper/AWS_Quicksight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\202112_AWS_AssociateDeveloper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706BAF59-0389-43F2-B09F-975195731235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA669B8-6B7C-4F1F-8A00-A326EC1D6DC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="S2.Basics" sheetId="3" r:id="rId3"/>
     <sheet name="S3.Data" sheetId="4" r:id="rId4"/>
     <sheet name="S4.Visualize" sheetId="5" r:id="rId5"/>
-    <sheet name="S5.Export" sheetId="6" r:id="rId6"/>
+    <sheet name="S5.Share" sheetId="6" r:id="rId6"/>
     <sheet name="S6.Database" sheetId="7" r:id="rId7"/>
     <sheet name="S7.Roundup" sheetId="8" r:id="rId8"/>
   </sheets>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="588">
   <si>
     <t>https://www.udemy.com/course/amazon-aws-quicksight-getting-started/learn/lecture/7234146</t>
   </si>
@@ -1869,9 +1869,6 @@
     </r>
   </si>
   <si>
-    <t>Story; Line chart; Treemap; Filter; Pivot tables; Heat maps; KPI visual;</t>
-  </si>
-  <si>
     <t>'region'</t>
   </si>
   <si>
@@ -2128,6 +2125,621 @@
   <si>
     <t>'revenue-total (SUM)'</t>
   </si>
+  <si>
+    <t>Story; Filter; Line chart; Treemap; Pivot tables; Heat maps; KPI visual;</t>
+  </si>
+  <si>
+    <t>Our ways to Continue</t>
+  </si>
+  <si>
+    <t>SPICE  - Finished analysis</t>
+  </si>
+  <si>
+    <t>Understanding Refresh and Schedule Refresh</t>
+  </si>
+  <si>
+    <t>We loaded data into SPICE.</t>
+  </si>
+  <si>
+    <t>It could be that we updated the file that we saved in S3 bucket.</t>
+  </si>
+  <si>
+    <t>We can only refresh data from some kind of AWS services (Ex. S3).</t>
+  </si>
+  <si>
+    <t>Refresh type</t>
+  </si>
+  <si>
+    <t>S3 Manifest</t>
+  </si>
+  <si>
+    <t>Full refresh</t>
+  </si>
+  <si>
+    <t>Existing manifest | Upload manifest | URL of manifest</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If we press </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>REFRESH NOW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =&gt; this data would again be loaded into SPICE.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SCHEDULE REFRESH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Create a schedule</t>
+    </r>
+  </si>
+  <si>
+    <t>Time zone</t>
+  </si>
+  <si>
+    <t>Repeats</t>
+  </si>
+  <si>
+    <t>Starting</t>
+  </si>
+  <si>
+    <t>At</t>
+  </si>
+  <si>
+    <t>Asia/Singapore</t>
+  </si>
+  <si>
+    <t>Daily | Weekly | Monthly</t>
+  </si>
+  <si>
+    <t>Export our Project Data as .csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open our analysis 'population-project'. </t>
+  </si>
+  <si>
+    <t>&gt; Select a visual &gt; Export to CSV</t>
+  </si>
+  <si>
+    <t>Create the first QuickSight project: Data set &amp; Visual</t>
+  </si>
+  <si>
+    <t>Adding Users to our Account</t>
+  </si>
+  <si>
+    <t>There are 2 types of users:</t>
+  </si>
+  <si>
+    <t>QuickSight only</t>
+  </si>
+  <si>
+    <t>Not AWS account, only email address.</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Type of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Role</t>
+    </r>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add additional SPICE space </t>
+  </si>
+  <si>
+    <t xml:space="preserve">QuickSight only user: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can work on subscription, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">add additional users to this account </t>
+  </si>
+  <si>
+    <t>IAM user:</t>
+  </si>
+  <si>
+    <t>Same as above.</t>
+  </si>
+  <si>
+    <t>Can access other AWS services.</t>
+  </si>
+  <si>
+    <t>Can delete the QuickSight account.</t>
+  </si>
+  <si>
+    <t>QuickSight &gt; Manage QuickSight &gt; Manage users &gt; Invite users</t>
+  </si>
+  <si>
+    <t>Type IAM user or email address</t>
+  </si>
+  <si>
+    <t>NOTE 1: Check the pricing before add users. It may charge $$$.</t>
+  </si>
+  <si>
+    <t>NOTE 2: At first the invited user CANNOT access our data sets.</t>
+  </si>
+  <si>
+    <t>Sharing our Data Set</t>
+  </si>
+  <si>
+    <t>Refresh; Schedule Refresh; Export CSV;</t>
+  </si>
+  <si>
+    <t>Can only create analysis based on the data set.</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Can edit the data set; refresh; share; delete;</t>
+  </si>
+  <si>
+    <t>QuickSight &gt; Manage data &gt; Select our 'project-stock' &gt; Share</t>
+  </si>
+  <si>
+    <t>Type a user name or email</t>
+  </si>
+  <si>
+    <t>Select Permission</t>
+  </si>
+  <si>
+    <t>Sharing our Analysis</t>
+  </si>
+  <si>
+    <t>Only share CO-OWNER permission. BE-AWARE!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User | </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Owner</t>
+    </r>
+  </si>
+  <si>
+    <t>Creating and Sharing Dashboard</t>
+  </si>
+  <si>
+    <t>READ-ONLY.</t>
+  </si>
+  <si>
+    <t>View; Export as CSV; Apply different filter;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Share all our </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>visuals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>underlying data behind</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that visuals.</t>
+    </r>
+  </si>
+  <si>
+    <t>Managing Capacity and Understand Subscriptions</t>
+  </si>
+  <si>
+    <t>Invite users; Share data set; Sharing Analysis; Sharing Dashboard;</t>
+  </si>
+  <si>
+    <t>IAM user</t>
+  </si>
+  <si>
+    <t>QuickSight &gt; Manage QuickSight &gt; Your Subscriptions</t>
+  </si>
+  <si>
+    <t>Readers</t>
+  </si>
+  <si>
+    <t>Per reader pricing</t>
+  </si>
+  <si>
+    <t>Monthly subscription</t>
+  </si>
+  <si>
+    <t>Up to $5/reader/month, $0.30/session.</t>
+  </si>
+  <si>
+    <t>Annual subscription</t>
+  </si>
+  <si>
+    <t>Start at $250/month</t>
+  </si>
+  <si>
+    <t>*1 session = 30 mins. from login</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Monthly billed users</t>
+  </si>
+  <si>
+    <t>1GB Free Tier</t>
+  </si>
+  <si>
+    <t>Purchase more capacity</t>
+  </si>
+  <si>
+    <t>Take a Quick Look at the Mobile App</t>
+  </si>
+  <si>
+    <t>SPICE Capacity; Subscription; Mobile App;</t>
+  </si>
+  <si>
+    <t>How to refresh data</t>
+  </si>
+  <si>
+    <t>Export to CSV file</t>
+  </si>
+  <si>
+    <t>Share our project</t>
+  </si>
+  <si>
+    <t>Invite users to QuickSight account</t>
+  </si>
+  <si>
+    <t>Share data set, analysis, dashboard</t>
+  </si>
+  <si>
+    <t>Subscription &amp; Pricing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can simply access QuickSight </t>
+  </si>
+  <si>
+    <t>but doesn’t have any kind of administrative roles</t>
+  </si>
+  <si>
+    <t>Rights depend on account type.</t>
+  </si>
+  <si>
+    <t>Setting up a Database</t>
+  </si>
+  <si>
+    <t>QuickSight can still connect to DB running in different region.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB Instance Security Group </t>
+  </si>
+  <si>
+    <t>DB Name</t>
+  </si>
+  <si>
+    <t>qs</t>
+  </si>
+  <si>
+    <t>rds-launch-wizard-1 (sg-cb1022a2)</t>
+  </si>
+  <si>
+    <t>Inbound/Outbound rule</t>
+  </si>
+  <si>
+    <t>Preparing Dummy Data</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>quicksight.cmt14yukspod.us-east-2.rds.amazonaws.com</t>
+  </si>
+  <si>
+    <t>Create RDS MySQL DB Instance</t>
+  </si>
+  <si>
+    <t>$ mysql -h [Endpoint] -P 3306 -u root -p</t>
+  </si>
+  <si>
+    <t>Connect to RDS MySQL DB Instance</t>
+  </si>
+  <si>
+    <t>Insert dummy data</t>
+  </si>
+  <si>
+    <t>create_fill_customers.sql</t>
+  </si>
+  <si>
+    <t>create_fill_orders.sql</t>
+  </si>
+  <si>
+    <t>create_fill_products.sql</t>
+  </si>
+  <si>
+    <t>Connecting QuickSight to a Database</t>
+  </si>
+  <si>
+    <t>QuickSight &gt; Manage QuickSight &gt; Security &amp; permissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access granted to Amazon RDS... </t>
+  </si>
+  <si>
+    <t>Database name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Step 1: Enable QuickSight access to AWS services</t>
+  </si>
+  <si>
+    <t>Step 2: Create new Security Group for QuickSight access RDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDS MySQL DB Instance Security Group </t>
+  </si>
+  <si>
+    <t>Security group name</t>
+  </si>
+  <si>
+    <t>rds-quicksight</t>
+  </si>
+  <si>
+    <t>VPC</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Inbound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom TCP rule; TCP; Port 3306; </t>
+  </si>
+  <si>
+    <t>https://docs.aws.amazon.com/quicksight/latest/user/regions.html</t>
+  </si>
+  <si>
+    <t>How do I find AWS QuickSight IP Range</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Source: Custom; CIDR = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>52.23.63.224/27</t>
+    </r>
+  </si>
+  <si>
+    <t>Add new security group to our DB instance.</t>
+  </si>
+  <si>
+    <t>quicksight-customer</t>
+  </si>
+  <si>
+    <t>Database server</t>
+  </si>
+  <si>
+    <t>QuickSight &gt; Manage data &gt; MySQL</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>More resources about connecting QuickSight to Databases</t>
+  </si>
+  <si>
+    <t>Creating a Database Data</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/quicksight/latest/user/create-a-database-data-set.html</t>
+  </si>
+  <si>
+    <t>Network &amp; Database Configuration</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/quicksight/latest/user/configure-access.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup DB; Connect QuickSight to DB; </t>
+  </si>
+  <si>
+    <t>Import Data to SPICE</t>
+  </si>
+  <si>
+    <t>Select more tables (customers, orders, products)</t>
+  </si>
+  <si>
+    <t>Configure join</t>
+  </si>
+  <si>
+    <t>Work with calculated fields</t>
+  </si>
+  <si>
+    <t>Set data set name</t>
+  </si>
+  <si>
+    <t>Import Data as a Query</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Validate connection &gt; Create data source &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Edit/Preview data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (to add more than 1 table)</t>
+    </r>
+  </si>
+  <si>
+    <t>NOTE: If we have to Join table, we must use SPICE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data source: SPICE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data source: Query </t>
+  </si>
+  <si>
+    <t>Select one table</t>
+  </si>
+  <si>
+    <t>Save an create analysis</t>
+  </si>
+  <si>
+    <t>Calculated Fields and Query Imports</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For importing data as a Query, we can </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>add calculated field on Analysis,</t>
+    </r>
+  </si>
+  <si>
+    <t>since this data is constantly pulled from DB.</t>
+  </si>
+  <si>
+    <t>What about NoSQL Databases?</t>
+  </si>
+  <si>
+    <t>There is no option to connect to NoSQL DB directly (Ex. DynamoDB).</t>
+  </si>
+  <si>
+    <t>We have to transfer it into Redshift, Datawarehouse, or SQL DB first.</t>
+  </si>
+  <si>
+    <t>Or, export to CSV and upload to S3.</t>
+  </si>
+  <si>
+    <t>Wrap Up</t>
+  </si>
+  <si>
+    <t>Connect QuickSight to SQL Database.</t>
+  </si>
+  <si>
+    <t>Import Data to SPICE; Import Data as a Query; Calculated Fields on Analysis;</t>
+  </si>
+  <si>
+    <t>Step 3: Connect QuickSight to RDS</t>
+  </si>
+  <si>
+    <t>QuickSight &gt; Manage QuickSight &gt; SPICE Capacity</t>
+  </si>
 </sst>
 </file>
 
@@ -2136,7 +2748,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2300,6 +2912,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2340,7 +2961,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2357,22 +2978,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4270,6 +4903,187 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>332876</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77247F15-32A5-43C4-BC70-DEAB31A3F6C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="1343025"/>
+          <a:ext cx="3990476" cy="1361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>256762</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>18857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0797754-22C2-498E-BE75-5CF020D26EC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="13725525"/>
+          <a:ext cx="3304762" cy="1542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>465981</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>161690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23BDED1A-C33B-49A5-B7C4-3A30D09F8DC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="11249025"/>
+          <a:ext cx="5952381" cy="1876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>46857</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>180786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{668A9990-E148-4BFB-A674-E0046CA77A6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="6677025"/>
+          <a:ext cx="6142857" cy="1514286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4535,8 +5349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4578,7 +5392,7 @@
       <c r="I6" s="2">
         <v>44620</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="26" t="s">
         <v>323</v>
       </c>
     </row>
@@ -4595,7 +5409,7 @@
       <c r="I7" s="2">
         <v>44620</v>
       </c>
-      <c r="J7" s="22"/>
+      <c r="J7" s="26"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -4610,7 +5424,7 @@
       <c r="I8" s="2">
         <v>44621</v>
       </c>
-      <c r="J8" s="22"/>
+      <c r="J8" s="26"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -4625,7 +5439,7 @@
       <c r="I9" s="2">
         <v>44622</v>
       </c>
-      <c r="J9" s="22"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -4640,7 +5454,7 @@
       <c r="I10" s="2">
         <v>44623</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="26"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -4653,9 +5467,9 @@
         <v>21</v>
       </c>
       <c r="I11" s="2">
-        <v>44624</v>
-      </c>
-      <c r="J11" s="22"/>
+        <v>44623</v>
+      </c>
+      <c r="J11" s="26"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -4668,9 +5482,9 @@
         <v>22</v>
       </c>
       <c r="I12" s="2">
-        <v>44625</v>
-      </c>
-      <c r="J12" s="22"/>
+        <v>44623</v>
+      </c>
+      <c r="J12" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4683,7 +5497,7 @@
     <hyperlink ref="H7" location="S2.Basics!A1" display="S2" xr:uid="{77D65065-E11B-459B-B364-F77F8EBDCF2C}"/>
     <hyperlink ref="H8" location="S3.Data!A1" display="S3" xr:uid="{B885BFAC-3A83-4C7C-A275-94B28C510824}"/>
     <hyperlink ref="H9" location="S4.Visualize!A1" display="S4" xr:uid="{6837F002-B192-4EE1-9C7E-00A778BD725D}"/>
-    <hyperlink ref="H10" location="S5.Export!A1" display="S5" xr:uid="{145EE37A-1387-42AA-892E-D36025A9CEA5}"/>
+    <hyperlink ref="H10" location="S5.Share!A1" display="S5" xr:uid="{145EE37A-1387-42AA-892E-D36025A9CEA5}"/>
     <hyperlink ref="H11" location="S6.Database!A1" display="S6" xr:uid="{4D7603A4-D960-4738-96B3-5DBF7E410806}"/>
     <hyperlink ref="H12" location="S7.Roundup!A1" display="S7" xr:uid="{5E8F40A4-0C8F-42D4-87C8-1508DF863539}"/>
   </hyperlinks>
@@ -4694,14 +5508,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB457A0-FC51-4A2C-B0E5-623DCCE18DCD}">
-  <dimension ref="B4:I60"/>
+  <dimension ref="B1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55:D56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>456</v>
+      </c>
+    </row>
     <row r="4" spans="2:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -5465,7 +6284,7 @@
       <c r="D71" t="s">
         <v>51</v>
       </c>
-      <c r="H71" s="20" t="s">
+      <c r="H71" s="18" t="s">
         <v>290</v>
       </c>
     </row>
@@ -5854,72 +6673,72 @@
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C152" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C154" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C157" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D158" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C159" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D160" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="161" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C161" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="162" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="163" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="164" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C164" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -5937,8 +6756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D3F9BD-4D98-448C-A713-F6EDB96ABCB8}">
   <dimension ref="B1:I211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I194" sqref="I194"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5950,7 +6769,7 @@
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>363</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="2:9" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -5967,16 +6786,16 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="G7" s="16" t="s">
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="G7" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -6003,10 +6822,10 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="16" t="s">
         <v>250</v>
       </c>
     </row>
@@ -6064,7 +6883,7 @@
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="18" t="s">
         <v>63</v>
       </c>
       <c r="E26" s="10" t="s">
@@ -6072,7 +6891,7 @@
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="22" t="s">
         <v>64</v>
       </c>
       <c r="E27" t="s">
@@ -6080,7 +6899,7 @@
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
         <v>261</v>
       </c>
       <c r="E28" t="s">
@@ -6133,7 +6952,7 @@
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="C41" s="29" t="s">
         <v>274</v>
       </c>
     </row>
@@ -6200,7 +7019,7 @@
       <c r="E50" t="s">
         <v>159</v>
       </c>
-      <c r="H50" s="19" t="s">
+      <c r="H50" s="17" t="s">
         <v>56</v>
       </c>
     </row>
@@ -6216,7 +7035,7 @@
       <c r="E52" t="s">
         <v>286</v>
       </c>
-      <c r="H52" s="20" t="s">
+      <c r="H52" s="18" t="s">
         <v>287</v>
       </c>
     </row>
@@ -6226,7 +7045,7 @@
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="18" t="s">
         <v>63</v>
       </c>
       <c r="E55" t="s">
@@ -6234,7 +7053,7 @@
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D56" s="25" t="s">
+      <c r="D56" s="22" t="s">
         <v>296</v>
       </c>
       <c r="E56" t="s">
@@ -6290,7 +7109,7 @@
       <c r="D68" t="s">
         <v>70</v>
       </c>
-      <c r="I68" s="21" t="s">
+      <c r="I68" s="19" t="s">
         <v>300</v>
       </c>
     </row>
@@ -6364,7 +7183,7 @@
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D83" s="20" t="s">
+      <c r="D83" s="18" t="s">
         <v>63</v>
       </c>
       <c r="E83" t="s">
@@ -6372,7 +7191,7 @@
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D84" s="25" t="s">
+      <c r="D84" s="22" t="s">
         <v>296</v>
       </c>
       <c r="E84" t="s">
@@ -6385,7 +7204,7 @@
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D86" s="20" t="s">
+      <c r="D86" s="18" t="s">
         <v>63</v>
       </c>
       <c r="E86" t="s">
@@ -6403,7 +7222,7 @@
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
+      <c r="C91" s="29" t="s">
         <v>326</v>
       </c>
     </row>
@@ -6480,7 +7299,7 @@
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C108" s="23" t="s">
+      <c r="C108" s="20" t="s">
         <v>353</v>
       </c>
     </row>
@@ -6575,7 +7394,7 @@
         <v>361</v>
       </c>
       <c r="E125" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="126" spans="2:8" x14ac:dyDescent="0.25">
@@ -6596,67 +7415,67 @@
     </row>
     <row r="128" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C128" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C129" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E133" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E134" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D135" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E136" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E137" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B139" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C140" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="142" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B142" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="143" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C143" s="24" t="s">
-        <v>381</v>
+      <c r="C143" s="21" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.25">
@@ -6666,12 +7485,12 @@
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D145" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C146" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
@@ -6679,7 +7498,7 @@
         <v>361</v>
       </c>
       <c r="E147" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
@@ -6687,7 +7506,7 @@
         <v>169</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
@@ -6695,47 +7514,47 @@
         <v>296</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="159" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B159" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="161" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C161" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="162" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="163" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="164" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C164" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="165" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D165" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="166" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C166" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="167" spans="3:6" x14ac:dyDescent="0.25">
@@ -6743,35 +7562,35 @@
         <v>64</v>
       </c>
       <c r="F167" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="168" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D168" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F168" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="169" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D169" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="171" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C171" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="172" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D172" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="173" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C173" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="174" spans="3:6" x14ac:dyDescent="0.25">
@@ -6779,66 +7598,66 @@
         <v>64</v>
       </c>
       <c r="F174" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="175" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D175" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F175" s="10"/>
     </row>
     <row r="176" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D176" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F176" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="178" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B178" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="179" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C179" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B181" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="183" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B183" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="184" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C184" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="185" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C185" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="186" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C186" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="187" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="188" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="189" spans="2:7" x14ac:dyDescent="0.25">
@@ -6846,7 +7665,7 @@
         <v>335</v>
       </c>
       <c r="G189" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="190" spans="2:7" x14ac:dyDescent="0.25">
@@ -6854,7 +7673,7 @@
         <v>333</v>
       </c>
       <c r="G190" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="191" spans="2:7" x14ac:dyDescent="0.25">
@@ -6873,17 +7692,17 @@
     </row>
     <row r="195" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C195" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="196" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D196" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="197" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D197" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="198" spans="3:7" x14ac:dyDescent="0.25">
@@ -6891,23 +7710,23 @@
         <v>63</v>
       </c>
       <c r="G198" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="199" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E199" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G199" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="200" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E200" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G200" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="201" spans="3:7" x14ac:dyDescent="0.25">
@@ -6915,30 +7734,30 @@
         <v>333</v>
       </c>
       <c r="G201" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="206" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C206" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="207" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D207" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="208" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D208" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="209" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E209" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G209" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="210" spans="5:7" x14ac:dyDescent="0.25">
@@ -6946,7 +7765,7 @@
         <v>169</v>
       </c>
       <c r="G210" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="211" spans="5:7" x14ac:dyDescent="0.25">
@@ -6954,7 +7773,7 @@
         <v>296</v>
       </c>
       <c r="G211" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -6970,14 +7789,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4075991E-4CC0-4B09-81A1-D873E17BA732}">
-  <dimension ref="B4:D4"/>
+  <dimension ref="B1:H111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>507</v>
+      </c>
+    </row>
     <row r="4" spans="2:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>8</v>
@@ -6986,22 +7820,431 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>441</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>442</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="18" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>447</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>448</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>449</v>
+      </c>
+      <c r="G28" s="24">
+        <v>44623</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>450</v>
+      </c>
+      <c r="G29" s="25">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="31" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D37" s="5" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="5" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="5" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E46" s="15" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C58" s="15" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C62" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="5" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="29" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>483</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C90" s="29" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
+        <v>496</v>
+      </c>
+      <c r="H92" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
+        <v>497</v>
+      </c>
+      <c r="H93" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E95" s="15" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C99" s="29" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>513</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00625B41-449D-4C4E-952B-A31EC4FE8449}">
-  <dimension ref="B4:D4"/>
+  <dimension ref="B1:H79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
@@ -7009,7 +8252,359 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>461</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>526</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>519</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="29" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="15" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>544</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>546</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>548</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="8" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D40" s="29" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>137</v>
+      </c>
+      <c r="H41" s="23" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>555</v>
+      </c>
+      <c r="H42" s="23" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>557</v>
+      </c>
+      <c r="H43" s="23">
+        <v>3306</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>538</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>539</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>540</v>
+      </c>
+      <c r="H46" s="23"/>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C61" s="30" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>584</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D36" r:id="rId1" xr:uid="{86B9060B-C59C-48D7-8558-67E8182890AA}"/>
+    <hyperlink ref="E51" r:id="rId2" xr:uid="{C3A76171-7E82-436E-A0EA-31CD5E99AE12}"/>
+    <hyperlink ref="E53" r:id="rId3" xr:uid="{1316504B-87DD-42AF-A913-21E59C262D26}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7019,7 +8614,7 @@
   <dimension ref="B4:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Practice on AWS QuickSight: Covid-19 data analysis
</commit_message>
<xml_diff>
--- a/202112_AWS_AssociateDeveloper/AWS_Quicksight.xlsx
+++ b/202112_AWS_AssociateDeveloper/AWS_Quicksight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\202112_AWS_AssociateDeveloper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA669B8-6B7C-4F1F-8A00-A326EC1D6DC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A71A5F-2387-4317-BB50-CBC1CB1DB30F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="689">
   <si>
     <t>https://www.udemy.com/course/amazon-aws-quicksight-getting-started/learn/lecture/7234146</t>
   </si>
@@ -2739,6 +2739,674 @@
   </si>
   <si>
     <t>QuickSight &gt; Manage QuickSight &gt; SPICE Capacity</t>
+  </si>
+  <si>
+    <t>Practice: Building a dynamic dashboard using QuickSight</t>
+  </si>
+  <si>
+    <t>Use public datasets to analyze Covid-19 data.</t>
+  </si>
+  <si>
+    <t>Covid-19 data:</t>
+  </si>
+  <si>
+    <t>Coordinates by Country:</t>
+  </si>
+  <si>
+    <t>https://ourworldindata.org/coronavirus-source-data</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/tadast/8827699</t>
+  </si>
+  <si>
+    <t>Step 1: Create data set</t>
+  </si>
+  <si>
+    <t>Import and join two data sources.</t>
+  </si>
+  <si>
+    <t>owid-covid-data.csv &amp; countries_codes_and_coordinates.csv</t>
+  </si>
+  <si>
+    <t>Step 2: Create analysis</t>
+  </si>
+  <si>
+    <t>Total Cases</t>
+  </si>
+  <si>
+    <t>Total Deaths</t>
+  </si>
+  <si>
+    <t>% Deaths / Cases</t>
+  </si>
+  <si>
+    <t>Create simple visual</t>
+  </si>
+  <si>
+    <t>new_cases (SUM)</t>
+  </si>
+  <si>
+    <t>date (DAY)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conditional formating</t>
+    </r>
+  </si>
+  <si>
+    <t>Different less than 0</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>Different greater or equal</t>
+  </si>
+  <si>
+    <t>Create Horizontal Bar chart</t>
+  </si>
+  <si>
+    <t>Total cases by region</t>
+  </si>
+  <si>
+    <t>new_deaths (SUM)</t>
+  </si>
+  <si>
+    <t>continent</t>
+  </si>
+  <si>
+    <t>Y axis drill-down layer</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Geospatial</t>
+  </si>
+  <si>
+    <t>NOTE: Geographical fields aren't supported in joins between data sources.</t>
+  </si>
+  <si>
+    <t>Need change type of 'latitude' &amp; 'longitude' from 'Decimal' to 'Latitude' and 'Longitude'</t>
+  </si>
+  <si>
+    <t>Latitude &amp; Longtitude</t>
+  </si>
+  <si>
+    <t>Create Point on Map visual (NOT HAVE GEOSPATIAL DATA)</t>
+  </si>
+  <si>
+    <t>Create Parameter</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>Static default value</t>
+  </si>
+  <si>
+    <t>New Cases</t>
+  </si>
+  <si>
+    <t>metricselection</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Single value</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> | Multiple values</t>
+    </r>
+  </si>
+  <si>
+    <t>Add Control</t>
+  </si>
+  <si>
+    <t>Display name</t>
+  </si>
+  <si>
+    <t>Metric To Display</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>Define specific values</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Specific values</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> | Link to dataset field</t>
+    </r>
+  </si>
+  <si>
+    <t>Total Cases; Total Cases per Million; Total Deaths; Total Deaths per Million;</t>
+  </si>
+  <si>
+    <r>
+      <t>ifelse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9B5000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>${metricselection}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF279392"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Total Cases'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9B5000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{new_cases}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9B5000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>${metricselection}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF279392"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Total Cases per Million'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9B5000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{new_cases_per_million}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9B5000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>${metricselection}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF279392"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Total Deaths'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9B5000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{new_deaths}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9B5000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{new_deaths_per_million}</t>
+    </r>
+  </si>
+  <si>
+    <t>    )</t>
+  </si>
+  <si>
+    <t>=&gt; Use 'Metric to Display (SUM)' in Horizontal Bar Chart; Point-on-Map chart;</t>
+  </si>
+  <si>
+    <t>Create KPI chart</t>
+  </si>
+  <si>
+    <t>sum({new_deaths}) / sum({new_cases})</t>
+  </si>
+  <si>
+    <r>
+      <t>Create new calculated filed '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Metric To Display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>':</t>
+    </r>
+  </si>
+  <si>
+    <t>Total cases / Total deaths over time trending</t>
+  </si>
+  <si>
+    <t>Create Clustered bar combo chart (Bar chart with line)</t>
+  </si>
+  <si>
+    <t>Bars</t>
+  </si>
+  <si>
+    <t>Group/Color for bars</t>
+  </si>
+  <si>
+    <t>Lines</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Metric to Display (SUM)</t>
+  </si>
+  <si>
+    <r>
+      <t>windowAvg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF2D29FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9B5000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{Metric to Display}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>), [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9B5000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF641B6B"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ASC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>], 7, 7)</t>
+    </r>
+  </si>
+  <si>
+    <t>Moving AVG (Custom)</t>
+  </si>
+  <si>
+    <t>Create moving average calculated field:</t>
+  </si>
+  <si>
+    <t>7 day before &amp; 7 day after</t>
+  </si>
+  <si>
+    <t>Add Date Filter</t>
+  </si>
+  <si>
+    <t>Date &amp; Time Range - Between</t>
+  </si>
+  <si>
+    <t>Time granularity</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Apply filter to some visuals:</t>
+  </si>
+  <si>
+    <t>Add Continent Filter</t>
+  </si>
+  <si>
+    <t>Apply to all visuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actions: </t>
+  </si>
+  <si>
+    <t>Custom action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url action: </t>
+  </si>
+  <si>
+    <t>re-directing to an external url</t>
+  </si>
+  <si>
+    <t>passing parameters of visual to the url</t>
+  </si>
+  <si>
+    <t>navigation action:</t>
+  </si>
+  <si>
+    <t>Sending us to a different sheet on our dashboard</t>
+  </si>
+  <si>
+    <t>filter action:</t>
+  </si>
+  <si>
+    <t>Apply to the whole dashboard</t>
+  </si>
+  <si>
+    <t>Create url action</t>
+  </si>
+  <si>
+    <t>https://wwwnc.cdc.gov/travel/notices/covid-4/coronavirus-france</t>
+  </si>
+  <si>
+    <t>Action name</t>
+  </si>
+  <si>
+    <t>Activation</t>
+  </si>
+  <si>
+    <t>See Travel Restrictions</t>
+  </si>
+  <si>
+    <t>Action type</t>
+  </si>
+  <si>
+    <t>URL action</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>{{base}}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select | </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Menu option</t>
+    </r>
+  </si>
+  <si>
+    <t>Open in</t>
+  </si>
+  <si>
+    <t>New browser tab</t>
+  </si>
+  <si>
+    <t>Update field 'location' to 'location no blank space'</t>
+  </si>
+  <si>
+    <t>replace({location}, ' ', '-');</t>
+  </si>
+  <si>
+    <t>Create Navigation action</t>
+  </si>
+  <si>
+    <t>Create Covid-19 dashboard</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MZGloAruLGQ</t>
   </si>
 </sst>
 </file>
@@ -2748,7 +3416,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2921,6 +3589,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2D29FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9B5000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF279392"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF641B6B"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2961,7 +3667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2994,6 +3700,9 @@
     <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3003,9 +3712,13 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5084,6 +5797,363 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>169599</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6150D82D-28B4-4656-8B5A-808F5E26D4E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705601" y="7629526"/>
+          <a:ext cx="1752600" cy="1503098"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>361951</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>184317</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8718CAE8-B4FD-48D9-B45A-3B57C6B76F48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705601" y="5343525"/>
+          <a:ext cx="2190750" cy="1327317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>163675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F830547E-8614-4E97-B306-0BDADC53953D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705601" y="3057526"/>
+          <a:ext cx="5029199" cy="1116174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>167560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43431044-D3B1-4565-8213-6D65DFF43B41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="4391025"/>
+          <a:ext cx="3419475" cy="1120060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>187581</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B3CE5FF-640C-46BA-82C0-ECF0807C60F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705601" y="11630025"/>
+          <a:ext cx="2286000" cy="1521081"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>96900</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6DA1E61-D0D0-47EA-B4EA-7D82D3D7867F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="13344525"/>
+          <a:ext cx="1925700" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>16487</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0C56E5C-E99B-4772-A9A5-1534CF646747}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="14487526"/>
+          <a:ext cx="1285875" cy="1730986"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>168555</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FD592ED-67A9-4E89-BDA9-D42F089C419C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="20774025"/>
+          <a:ext cx="8915400" cy="4550055"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5349,7 +6419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -5392,7 +6462,7 @@
       <c r="I6" s="2">
         <v>44620</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="29" t="s">
         <v>323</v>
       </c>
     </row>
@@ -5409,7 +6479,7 @@
       <c r="I7" s="2">
         <v>44620</v>
       </c>
-      <c r="J7" s="26"/>
+      <c r="J7" s="29"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -5424,7 +6494,7 @@
       <c r="I8" s="2">
         <v>44621</v>
       </c>
-      <c r="J8" s="26"/>
+      <c r="J8" s="29"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -5439,7 +6509,7 @@
       <c r="I9" s="2">
         <v>44622</v>
       </c>
-      <c r="J9" s="26"/>
+      <c r="J9" s="29"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -5454,7 +6524,7 @@
       <c r="I10" s="2">
         <v>44623</v>
       </c>
-      <c r="J10" s="26"/>
+      <c r="J10" s="29"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -5469,7 +6539,7 @@
       <c r="I11" s="2">
         <v>44623</v>
       </c>
-      <c r="J11" s="26"/>
+      <c r="J11" s="29"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -5484,7 +6554,7 @@
       <c r="I12" s="2">
         <v>44623</v>
       </c>
-      <c r="J12" s="26"/>
+      <c r="J12" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6786,16 +7856,16 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="G7" s="27" t="s">
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="G7" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -6952,7 +8022,7 @@
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="26" t="s">
         <v>274</v>
       </c>
     </row>
@@ -7222,7 +8292,7 @@
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="29" t="s">
+      <c r="C91" s="26" t="s">
         <v>326</v>
       </c>
     </row>
@@ -7919,7 +8989,7 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="28" t="s">
         <v>455</v>
       </c>
     </row>
@@ -8064,7 +9134,7 @@
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C67" s="29" t="s">
+      <c r="C67" s="26" t="s">
         <v>481</v>
       </c>
     </row>
@@ -8117,7 +9187,7 @@
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C90" s="29" t="s">
+      <c r="C90" s="26" t="s">
         <v>494</v>
       </c>
     </row>
@@ -8163,7 +9233,7 @@
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C99" s="29" t="s">
+      <c r="C99" s="26" t="s">
         <v>587</v>
       </c>
     </row>
@@ -8350,7 +9420,7 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="26" t="s">
         <v>536</v>
       </c>
     </row>
@@ -8419,7 +9489,7 @@
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="29" t="s">
+      <c r="D40" s="26" t="s">
         <v>556</v>
       </c>
     </row>
@@ -8530,7 +9600,7 @@
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C61" s="30" t="s">
+      <c r="C61" s="27" t="s">
         <v>571</v>
       </c>
     </row>
@@ -8611,15 +9681,25 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D4AC902-4CE2-4FA7-91F2-000191C16CCE}">
-  <dimension ref="B4:D4"/>
+  <dimension ref="B1:I107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
@@ -8627,7 +9707,518 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>591</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>595</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="32" t="s">
+        <v>616</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>617</v>
+      </c>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>598</v>
+      </c>
+      <c r="H18" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>599</v>
+      </c>
+      <c r="H19" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>600</v>
+      </c>
+      <c r="H20" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>389</v>
+      </c>
+      <c r="H26" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>605</v>
+      </c>
+      <c r="H28" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>608</v>
+      </c>
+      <c r="H29" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>424</v>
+      </c>
+      <c r="H33" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>613</v>
+      </c>
+      <c r="H36" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="32" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>615</v>
+      </c>
+      <c r="H39" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C43" s="4" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>621</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>622</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>296</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>623</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>628</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>630</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>296</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>632</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E54" s="33" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E55" s="34" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E56" s="34" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E57" s="34" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E58" s="34" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E59" s="34" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D60" s="10" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C62" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H63" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>647</v>
+      </c>
+      <c r="H64" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>649</v>
+      </c>
+      <c r="H66" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="67" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E69" s="33" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C71" s="4" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="72" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="74" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>658</v>
+      </c>
+      <c r="I74" s="8" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="77" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C77" s="4" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="78" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C87" s="4" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E89" s="5" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E92" s="5" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E94" s="5" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="97" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="98" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E98" s="1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="99" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
+        <v>674</v>
+      </c>
+      <c r="I99" s="8" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="100" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E100" t="s">
+        <v>675</v>
+      </c>
+      <c r="I100" s="8" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="101" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E101" t="s">
+        <v>677</v>
+      </c>
+      <c r="I101" s="8" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="102" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>679</v>
+      </c>
+      <c r="I102" s="8" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="103" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E103" t="s">
+        <v>682</v>
+      </c>
+      <c r="I103" s="8" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="104" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="105" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E105" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="107" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>686</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{C879E5A0-2A8C-469C-988A-5DC11A5C73DE}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{0BA46BB8-9332-435B-85D7-6E9DB70EC63F}"/>
+    <hyperlink ref="E98" r:id="rId3" xr:uid="{85ADC441-2581-4C6E-940C-04454C5C2317}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{E79AE11E-C97A-481E-BC87-D90162AA13DF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>